<commit_message>
update bin rang table
</commit_message>
<xml_diff>
--- a/resource/test_bin_peak.xlsx
+++ b/resource/test_bin_peak.xlsx
@@ -28,12 +28,12 @@
     <t xml:space="preserve">gene</t>
   </si>
   <si>
+    <t xml:space="preserve">marker_label</t>
+  </si>
+  <si>
     <t xml:space="preserve">marker</t>
   </si>
   <si>
-    <t xml:space="preserve">marker_label</t>
-  </si>
-  <si>
     <t xml:space="preserve">is_forward</t>
   </si>
   <si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">m_color</t>
   </si>
   <si>
-    <t xml:space="preserve">CYP2D6-S1</t>
+    <t xml:space="preserve">S1</t>
   </si>
   <si>
     <t xml:space="preserve">CYP2D6</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">CYP2D6_010</t>
   </si>
   <si>
-    <t xml:space="preserve">CYP2D6-S2</t>
+    <t xml:space="preserve">S2</t>
   </si>
   <si>
     <t xml:space="preserve">CYP2D6_4</t>
@@ -209,6 +209,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -253,6 +254,7 @@
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -355,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,10 +370,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,10 +398,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,10 +428,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -552,12 +542,14 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,33 +568,33 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -614,687 +606,704 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="7" t="b">
+      <c r="E2" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="b">
+      <c r="E3" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="9" t="n">
         <v>38</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="9" t="n">
         <v>31</v>
       </c>
-      <c r="I3" s="10" t="n">
+      <c r="I3" s="9" t="n">
         <v>37</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="7" t="b">
+      <c r="E4" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="9" t="n">
         <v>37</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G4" s="9" t="n">
         <v>44</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="9" t="n">
         <v>39</v>
       </c>
-      <c r="I4" s="10" t="n">
+      <c r="I4" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="b">
+      <c r="E5" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="9" t="n">
         <v>41</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="9" t="n">
         <v>42</v>
       </c>
-      <c r="I5" s="10" t="n">
+      <c r="I5" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="7" t="b">
+      <c r="E6" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="H6" s="9" t="n">
         <v>47</v>
       </c>
-      <c r="I6" s="10" t="n">
+      <c r="I6" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="7" t="b">
+      <c r="E7" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="9" t="n">
         <v>53</v>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="I7" s="10" t="n">
+      <c r="I7" s="9" t="n">
         <v>55</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7" t="b">
+      <c r="E8" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="9" t="n">
         <v>53</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G8" s="9" t="n">
         <v>57</v>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="9" t="n">
         <v>55</v>
       </c>
-      <c r="I8" s="10" t="n">
+      <c r="I8" s="9" t="n">
         <v>59</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="7" t="b">
+      <c r="E9" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="10" t="n">
+      <c r="F9" s="9" t="n">
         <v>57</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="9" t="n">
         <v>62</v>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="H9" s="9" t="n">
         <v>59</v>
       </c>
-      <c r="I9" s="10" t="n">
+      <c r="I9" s="9" t="n">
         <v>63</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="7" t="b">
+      <c r="E10" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="9" t="n">
         <v>63</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="G10" s="9" t="n">
         <v>68</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="9" t="n">
         <v>65</v>
       </c>
-      <c r="I10" s="10" t="n">
+      <c r="I10" s="9" t="n">
         <v>68</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="7" t="b">
+      <c r="E11" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F11" s="20" t="n">
+      <c r="F11" s="16" t="n">
         <v>68</v>
       </c>
-      <c r="G11" s="20" t="n">
+      <c r="G11" s="16" t="n">
         <v>73</v>
       </c>
-      <c r="H11" s="20" t="n">
+      <c r="H11" s="16" t="n">
         <v>68</v>
       </c>
-      <c r="I11" s="20" t="n">
+      <c r="I11" s="16" t="n">
         <v>72</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="b">
+      <c r="E12" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="G12" s="3" t="n">
+      <c r="G12" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="b">
+      <c r="E13" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="9" t="n">
         <v>33</v>
       </c>
-      <c r="G13" s="10" t="n">
+      <c r="G13" s="9" t="n">
         <v>38</v>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="9" t="n">
         <v>32</v>
       </c>
-      <c r="I13" s="10" t="n">
+      <c r="I13" s="9" t="n">
         <v>36</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="M13" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="7" t="b">
+      <c r="E14" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="9" t="n">
         <v>36</v>
       </c>
-      <c r="G14" s="10" t="n">
+      <c r="G14" s="9" t="n">
         <v>41</v>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="9" t="n">
         <v>38</v>
       </c>
-      <c r="I14" s="10" t="n">
+      <c r="I14" s="9" t="n">
         <v>43</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="13" t="s">
+      <c r="M14" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="7" t="b">
+      <c r="E15" s="6" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="9" t="n">
         <v>41</v>
       </c>
-      <c r="G15" s="10" t="n">
+      <c r="G15" s="9" t="n">
         <v>46</v>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="9" t="n">
         <v>39</v>
       </c>
-      <c r="I15" s="10" t="n">
+      <c r="I15" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="14" t="s">
+      <c r="L15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="25" t="s">
+      <c r="M15" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="7" t="b">
+      <c r="E16" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="G16" s="10" t="n">
+      <c r="G16" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="9" t="n">
         <v>46</v>
       </c>
-      <c r="I16" s="10" t="n">
+      <c r="I16" s="9" t="n">
         <v>49</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="7" t="b">
+      <c r="E17" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="G17" s="9" t="n">
         <v>55</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="9" t="n">
         <v>52</v>
       </c>
-      <c r="I17" s="10" t="n">
+      <c r="I17" s="9" t="n">
         <v>57</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="M17" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="26" t="s">
+      <c r="B18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="7" t="b">
+      <c r="E18" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F18" s="20" t="n">
+      <c r="F18" s="16" t="n">
         <v>66</v>
       </c>
-      <c r="G18" s="20" t="n">
+      <c r="G18" s="16" t="n">
         <v>73</v>
       </c>
-      <c r="H18" s="20" t="n">
+      <c r="H18" s="16" t="n">
         <v>70</v>
       </c>
-      <c r="I18" s="20" t="n">
+      <c r="I18" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="27" t="s">
+      <c r="L18" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="28" t="s">
+      <c r="M18" s="25" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated definition tables
</commit_message>
<xml_diff>
--- a/resource/test_bin_peak.xlsx
+++ b/resource/test_bin_peak.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t xml:space="preserve">panel</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">m_color</t>
   </si>
   <si>
+    <t xml:space="preserve">w_height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_height</t>
+  </si>
+  <si>
     <t xml:space="preserve">S1</t>
   </si>
   <si>
@@ -79,10 +85,10 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">파랑</t>
-  </si>
-  <si>
-    <t xml:space="preserve">초록</t>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
   </si>
   <si>
     <t xml:space="preserve">CYP2D6_10B</t>
@@ -97,10 +103,10 @@
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve">검정</t>
-  </si>
-  <si>
-    <t xml:space="preserve">빨강</t>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
   </si>
   <si>
     <t xml:space="preserve">CYP2D6_49</t>
@@ -204,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -248,6 +254,13 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -357,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -382,6 +395,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,7 +415,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -406,18 +435,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -430,11 +447,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -454,11 +467,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,15 +548,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
   </cols>
@@ -592,21 +601,27 @@
       <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
+      <c r="A2" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -623,410 +638,470 @@
         <v>36</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>21</v>
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="H3" s="9" t="n">
+      <c r="H3" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="L3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>27</v>
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="G4" s="9" t="n">
+      <c r="G4" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="H4" s="9" t="n">
+      <c r="H4" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="I4" s="9" t="n">
+      <c r="I4" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="12" t="s">
+      <c r="J4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>26</v>
+      <c r="L4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>29</v>
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E5" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <v>41</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="10" t="n">
         <v>42</v>
       </c>
-      <c r="I5" s="9" t="n">
+      <c r="I5" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="K5" s="10" t="s">
         <v>25</v>
       </c>
+      <c r="L5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>31</v>
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="E6" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="13" t="s">
+      <c r="J6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="K6" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="L6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>33</v>
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="I7" s="9" t="n">
+      <c r="I7" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>26</v>
+      <c r="J7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>35</v>
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="E8" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="G8" s="9" t="n">
+      <c r="G8" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="H8" s="9" t="n">
+      <c r="H8" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="I8" s="9" t="n">
+      <c r="I8" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="13" t="s">
+      <c r="J8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="L8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>37</v>
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="E9" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="10" t="n">
         <v>62</v>
       </c>
-      <c r="H9" s="9" t="n">
+      <c r="H9" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="10" t="n">
         <v>63</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>20</v>
+      <c r="J9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>39</v>
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="E10" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="10" t="n">
         <v>63</v>
       </c>
-      <c r="G10" s="9" t="n">
+      <c r="G10" s="10" t="n">
         <v>68</v>
       </c>
-      <c r="H10" s="9" t="n">
+      <c r="H10" s="10" t="n">
         <v>65</v>
       </c>
-      <c r="I10" s="9" t="n">
+      <c r="I10" s="10" t="n">
         <v>68</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>26</v>
+      <c r="J10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>41</v>
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="E11" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F11" s="16" t="n">
+      <c r="F11" s="17" t="n">
         <v>68</v>
       </c>
-      <c r="G11" s="16" t="n">
+      <c r="G11" s="17" t="n">
         <v>73</v>
       </c>
-      <c r="H11" s="16" t="n">
+      <c r="H11" s="17" t="n">
         <v>68</v>
       </c>
-      <c r="I11" s="16" t="n">
+      <c r="I11" s="17" t="n">
         <v>72</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>26</v>
+      <c r="J11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>43</v>
+      <c r="A12" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="6" t="n">
+        <v>47</v>
+      </c>
+      <c r="E12" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1043,268 +1118,310 @@
         <v>34</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>14</v>
+      <c r="A13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="E13" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="G13" s="9" t="n">
+      <c r="G13" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="H13" s="9" t="n">
+      <c r="H13" s="10" t="n">
         <v>32</v>
       </c>
-      <c r="I13" s="9" t="n">
+      <c r="I13" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="J13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="12" t="s">
+      <c r="J13" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="K13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="M13" s="22" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>14</v>
+      <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="E14" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="G14" s="9" t="n">
+      <c r="G14" s="10" t="n">
         <v>41</v>
       </c>
-      <c r="H14" s="9" t="n">
+      <c r="H14" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="I14" s="9" t="n">
+      <c r="I14" s="10" t="n">
         <v>43</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" s="10" t="s">
+      <c r="J14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="L14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>14</v>
+      <c r="A15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="E15" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="10" t="n">
         <v>41</v>
       </c>
-      <c r="G15" s="9" t="n">
+      <c r="G15" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="H15" s="9" t="n">
+      <c r="H15" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="I15" s="9" t="n">
+      <c r="I15" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="12" t="s">
+      <c r="J15" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="K15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="M15" s="22" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>14</v>
+      <c r="A16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="E16" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F16" s="9" t="n">
+      <c r="F16" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="G16" s="9" t="n">
+      <c r="G16" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="H16" s="9" t="n">
+      <c r="H16" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="I16" s="9" t="n">
+      <c r="I16" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="14" t="s">
-        <v>25</v>
+      <c r="J16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>14</v>
+      <c r="A17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="E17" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F17" s="9" t="n">
+      <c r="F17" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="G17" s="9" t="n">
+      <c r="G17" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="H17" s="9" t="n">
+      <c r="H17" s="10" t="n">
         <v>52</v>
       </c>
-      <c r="I17" s="9" t="n">
+      <c r="I17" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>26</v>
+      <c r="J17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>14</v>
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="E18" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F18" s="16" t="n">
+      <c r="F18" s="17" t="n">
         <v>66</v>
       </c>
-      <c r="G18" s="16" t="n">
+      <c r="G18" s="17" t="n">
         <v>73</v>
       </c>
-      <c r="H18" s="16" t="n">
+      <c r="H18" s="17" t="n">
         <v>70</v>
       </c>
-      <c r="I18" s="16" t="n">
+      <c r="I18" s="17" t="n">
         <v>75</v>
       </c>
-      <c r="J18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>18</v>
+      <c r="J18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>